<commit_message>
a happy commit: using dict to handle data... its more professional and pythonical
</commit_message>
<xml_diff>
--- a/data/login/valid_login.xlsx
+++ b/data/login/valid_login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Teste" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
@@ -41,7 +41,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +51,20 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -79,11 +93,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -392,16 +409,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -423,19 +440,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>